<commit_message>
Clean up git repo and update readme
</commit_message>
<xml_diff>
--- a/simulation_setups/multi_carve/Simulations.xlsx
+++ b/simulation_setups/multi_carve/Simulations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackheller/KU/Thesis/Thesis/simulation_setups/multi_carve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBAA12C0-7B50-4B87-915D-AB7150B5B733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C37BEF65-B791-4A72-959E-61C22D91C150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="170">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>NActive</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
   <si>
     <t>23.03.23</t>
@@ -122,6 +128,9 @@
     <t>Viki</t>
   </si>
   <si>
+    <t>Logit</t>
+  </si>
+  <si>
     <t>26.03.23</t>
   </si>
   <si>
@@ -210,6 +219,9 @@
     <t>Jack</t>
   </si>
   <si>
+    <t>cloglog</t>
+  </si>
+  <si>
     <t>19.04.23</t>
   </si>
   <si>
@@ -713,16 +725,47 @@
 nsim &lt;- 100</t>
   </si>
   <si>
-    <t>04.04.23</t>
-  </si>
-  <si>
-    <t>00.17</t>
-  </si>
-  <si>
-    <t>00.17 to 06.12</t>
+    <t>28.04.23</t>
+  </si>
+  <si>
+    <t>23.48</t>
+  </si>
+  <si>
+    <t>jack already ran f=0.5,0.75</t>
+  </si>
+  <si>
+    <t>Change correlation to 0.9</t>
+  </si>
+  <si>
+    <t>24.04.23</t>
+  </si>
+  <si>
+    <t>15.26</t>
+  </si>
+  <si>
+    <t>f=0.95 Failed so redoing f=0.95, 0.99 on the 25.04, 7:48</t>
   </si>
   <si>
     <t>Investigate different # of actives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n = 100
+p = 200
+rho = 0
+B = 1, 5, 10, 20, 50
+f = 0.5, 0.75, 0.9, 0.95, 0.99
+nsim=100
+link = logit
+#active = 5 </t>
+  </si>
+  <si>
+    <t>23.04.23</t>
+  </si>
+  <si>
+    <t>17.05</t>
+  </si>
+  <si>
+    <t>17.00-01.00</t>
   </si>
   <si>
     <t>n = 100
@@ -759,44 +802,6 @@
   <si>
     <t>n = 100
 p = 200
-rho = 0.6
-B = 1, 5, 10, 20, 50
-f = 0.5, 0.75, 0.9, 0.95, 0.99
-nsim=100
-link = logit
-#active = 10</t>
-  </si>
-  <si>
-    <t># toeplitz
-n &lt;- 100
-p &lt;- 200
-rho &lt;- 0.6
-level&lt;-0.05 #17/02/23 VK, setting significance level only once
-Cov &lt;- toeplitz(rho ^ (seq(0, p - 1)))
-sel.index &lt;- c(1, 21, 41, 61, 81, 101, 121, 141, 161, 181)
-ind &lt;- sel.index
-beta &lt;- rep(0, p)
-beta[sel.index] &lt;- 1
-sparsity &lt;- length(sel.index) # 17/02/23 VK, changed so that value automatically updates
-set.seed(42) # to make different methods comparable, fix the x-matrix
-x &lt;- mvrnorm(n, rep(0, p), Cov)
-print (x[1,1])
-# should create the right x on D-MATH server, x[1 ,1] = 0.958
-xb &lt;- x %*% beta
-p.true &lt;- exp(xb) / (1 + exp(xb))
-B.vec &lt;- c(1, 5, 10, 20, 50) # c(1, (1:5) * 10) # number of splits
-frac.vec &lt;- c(0.5, 0.75, 0.9, 0.95, 0.99) # selection fraction
-nsim &lt;- 100</t>
-  </si>
-  <si>
-    <t>05.04.23</t>
-  </si>
-  <si>
-    <t>01.44 to 07.17</t>
-  </si>
-  <si>
-    <t>n = 100
-p = 200
 rho = 0
 B = 1, 5, 10, 20, 50
 f = 0.5, 0.75, 0.9, 0.95, 0.99
@@ -827,7 +832,10 @@
 nsim &lt;- 100</t>
   </si>
   <si>
-    <t xml:space="preserve">computer went to sleep so I had to continue in the morning </t>
+    <t>26.04.23</t>
+  </si>
+  <si>
+    <t>contains all except f=0.95 so far</t>
   </si>
   <si>
     <t>n = 100
@@ -845,7 +853,7 @@
 rho &lt;- 0
 level&lt;-0.05 #17/02/23 VK, setting significance level only once
 Cov &lt;- toeplitz(rho ^ (seq(0, p - 1)))
-sel.index &lt;- c(1, 5, 10, 15, 20, 25, 30, 35, 40, 45)
+sel.index &lt;- c(1, 3, 5, 7, 9, 11, 13, 15, 17, 19)
 ind &lt;- sel.index
 beta &lt;- rep(0, p)
 beta[sel.index] &lt;- 2
@@ -875,13 +883,129 @@
 #active = 5</t>
   </si>
   <si>
-    <t>carving_betabinomial_simulation</t>
-  </si>
-  <si>
-    <t>Investigate beta binomial. Not ready!!!</t>
-  </si>
-  <si>
-    <t>maybe at some point rerun for beta=0.5</t>
+    <t>11.05.23</t>
+  </si>
+  <si>
+    <t>around 6 hours</t>
+  </si>
+  <si>
+    <t>carving_binomial_simulation_betabinomoal</t>
+  </si>
+  <si>
+    <t>Beta Binomial, rho=0.3. Old simulation moved to old sims. Was 29.04.23 at 17.36</t>
+  </si>
+  <si>
+    <t># toeplitz
+n &lt;- 100
+p &lt;- 200
+rho &lt;- 0
+level&lt;-0.05 #17/02/23 VK, setting significance level only once
+Cov &lt;- toeplitz(rho ^ (seq(0, p - 1)))
+sel.index &lt;- c(1, 5, 10, 15, 20)
+ind &lt;- sel.index
+beta &lt;- rep(0, p)
+beta[sel.index] &lt;- 2
+sparsity &lt;- length(sel.index) # 17/02/23 VK, changed so that value automatically updates
+set.seed(42) # to make different methods comparable, fix the x-matrix
+x &lt;- mvrnorm(n, rep(0, p), Cov)
+print (x[1,1])
+# should create the right x on D-MATH server, x[1 ,1] = 0.958
+xb &lt;- x %*% beta
+p.true &lt;- exp(xb) / (1 + exp(xb))
+y &lt;- rbetabinom(n/10, 10, p.true, rho = 0.3)</t>
+  </si>
+  <si>
+    <t>bbinom03</t>
+  </si>
+  <si>
+    <t>06.05.23</t>
+  </si>
+  <si>
+    <t>DUPLICATE!</t>
+  </si>
+  <si>
+    <t>Beta Binomial, rho=0.3</t>
+  </si>
+  <si>
+    <t># toeplitz
+n &lt;- 100
+p &lt;- 200
+rho &lt;- 0
+level&lt;-0.05 #17/02/23 VK, setting significance level only once
+Cov &lt;- toeplitz(rho ^ (seq(0, p - 1)))
+sel.index &lt;- c(1, 5, 10, 15, 20)
+ind &lt;- sel.index
+beta &lt;- rep(0, p)
+beta[sel.index] &lt;- 2
+sparsity &lt;- length(sel.index) # 17/02/23 VK, changed so that value automatically updates
+set.seed(42) # to make different methods comparable, fix the x-matrix
+x &lt;- mvrnorm(n, rep(0, p), Cov)
+print (x[1,1])
+# should create the right x on D-MATH server, x[1 ,1] = 0.958
+xb &lt;- x %*% beta
+p.true &lt;- exp(xb) / (1 + exp(xb))
+y &lt;- rbetabinom(n, 1, p.true, rho = 0.3)</t>
+  </si>
+  <si>
+    <t>30.04.23</t>
+  </si>
+  <si>
+    <t>less than 5 hours!</t>
+  </si>
+  <si>
+    <t>rho=0.8</t>
+  </si>
+  <si>
+    <t>n = 100
+p = 200
+rho = 0.8
+B = 1, 5, 10, 20, 50
+f = 0.5, 0.75, 0.9, 0.95, 0.99
+nsim=100
+link = logit
+#active = 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+# toeplitz
+n &lt;- 100
+p &lt;- 200
+rho &lt;- 0.8
+level&lt;-0.05 #17/02/23 VK, setting significance level only once
+Cov &lt;- toeplitz(rho ^ (seq(0, p - 1)))
+sel.index &lt;- c(1, 5, 10, 15, 20)
+ind &lt;- sel.index
+beta &lt;- rep(0, p)
+beta[sel.index] &lt;- 2
+sparsity &lt;- length(sel.index) # 17/02/23 VK, changed so that value automatically updates
+set.seed(42) # to make different methods comparable, fix the x-matrix
+x &lt;- mvrnorm(n, rep(0, p), Cov)
+print (x[1,1])
+# should create the right x on D-MATH server, x[1 ,1] = 0.958
+xb &lt;- x %*% beta
+p.true &lt;- exp(xb) / (1 + exp(xb))
+B.vec &lt;- c(1, 5, 10, 20, 50) # c(1, (1:5) * 10) # number of splits
+frac.vec &lt;- c(0.5, 0.75, 0.9, 0.95, 0.99) # selection fraction
+nsim &lt;- 100
+</t>
+  </si>
+  <si>
+    <t>logit</t>
+  </si>
+  <si>
+    <t>04.05.23</t>
+  </si>
+  <si>
+    <t>carving_loanapp</t>
+  </si>
+  <si>
+    <t>200 rows
+Remove linear combinations
+Use lambda min
+nsim = 2</t>
+  </si>
+  <si>
+    <t>00.42</t>
   </si>
   <si>
     <t>Comuputation time</t>
@@ -1081,7 +1205,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,8 +1228,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1115,6 +1246,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,7 +1274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1149,29 +1292,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
     <dxf>
       <alignment horizontal="left" vertical="top"/>
     </dxf>
@@ -1201,6 +1361,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1294,21 +1466,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD2C4D0A-D055-47B5-B781-354F6AC7036D}" name="Table2" displayName="Table2" ref="A1:L23" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:L23" xr:uid="{AD2C4D0A-D055-47B5-B781-354F6AC7036D}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{DB21F81F-8454-4455-BB8B-39BDDD2B11EE}" name="Date" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{7D954777-7EA9-4A34-8D39-D16F57EE9258}" name="Time" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{01F05258-F571-48E3-9BC8-F0EF79316A89}" name="Run Time" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{0D1E676E-7661-49B6-870A-CE14DB4B922C}" name="Script" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{26E2BE03-EBAF-40D1-B950-7FCDB148FAD7}" name="Notes" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{67C6075F-027E-4FFB-9AE3-1BD2BC4F9B9D}" name="Settings" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{C6867D23-487A-4468-A5BD-AC16AD5539E7}" name="Code Snippet" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{C8246817-F368-DC42-AC09-84F98B285099}" name="Who will Run" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{85F0A740-AFC5-444E-A340-B5E851D6B8B0}" name="n" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{FBF5D462-50A3-4DB2-B674-2A9C88EA62F0}" name="p" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{75F9989C-BD10-46C9-A600-155B840B7CC8}" name="Coefficient" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{A768D360-FD94-4BB9-A42D-E0C465BA2FD8}" name="NActive" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AD2C4D0A-D055-47B5-B781-354F6AC7036D}" name="Table2" displayName="Table2" ref="A1:N26" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:N26" xr:uid="{AD2C4D0A-D055-47B5-B781-354F6AC7036D}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{DB21F81F-8454-4455-BB8B-39BDDD2B11EE}" name="Date" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7D954777-7EA9-4A34-8D39-D16F57EE9258}" name="Time" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{01F05258-F571-48E3-9BC8-F0EF79316A89}" name="Run Time" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{0D1E676E-7661-49B6-870A-CE14DB4B922C}" name="Script" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{26E2BE03-EBAF-40D1-B950-7FCDB148FAD7}" name="Notes" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{67C6075F-027E-4FFB-9AE3-1BD2BC4F9B9D}" name="Settings" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{C6867D23-487A-4468-A5BD-AC16AD5539E7}" name="Code Snippet" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{C8246817-F368-DC42-AC09-84F98B285099}" name="Who will Run" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{85F0A740-AFC5-444E-A340-B5E851D6B8B0}" name="n" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{FBF5D462-50A3-4DB2-B674-2A9C88EA62F0}" name="p" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{75F9989C-BD10-46C9-A600-155B840B7CC8}" name="Coefficient" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{A768D360-FD94-4BB9-A42D-E0C465BA2FD8}" name="NActive" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{681E9BC8-B62D-422A-9D3E-8B1DCFCD0D18}" name="Correlation" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{E56BDE22-A3BB-457E-849B-960DFBF3299A}" name="Link" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1629,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1643,9 +1817,10 @@
     <col min="5" max="5" width="57.140625" customWidth="1"/>
     <col min="6" max="6" width="30.85546875" customWidth="1"/>
     <col min="7" max="7" width="77" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" customHeight="1">
+    <row r="1" spans="1:14" ht="13.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1682,31 +1857,37 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="142.5" customHeight="1">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="142.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2">
         <v>100</v>
@@ -1720,31 +1901,37 @@
       <c r="L2" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="142.5" customHeight="1">
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="142.5" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="I3" s="2">
         <v>100</v>
@@ -1754,31 +1941,33 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" ht="142.5" customHeight="1">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="142.5" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I4" s="2">
         <v>100</v>
@@ -1790,99 +1979,107 @@
         <v>2</v>
       </c>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="209.25" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="366">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="7">
+      <c r="I5" s="2">
         <v>50</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="2">
         <v>200</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="142.5" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="7">
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="2">
         <v>100</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="2">
         <v>133</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="2">
         <v>2</v>
       </c>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="142.5" customHeight="1">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="142.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I7" s="2">
         <v>100</v>
@@ -1894,31 +2091,33 @@
         <v>5</v>
       </c>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" ht="142.5" customHeight="1">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="142.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I8" s="2">
         <v>100</v>
@@ -1930,29 +2129,31 @@
         <v>2</v>
       </c>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" ht="142.5" customHeight="1">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" ht="142.5" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I9" s="2">
         <v>100</v>
@@ -1964,29 +2165,31 @@
         <v>7.5</v>
       </c>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="142.5" customHeight="1">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" s="4" customFormat="1" ht="142.5" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I10" s="2">
         <v>100</v>
@@ -1998,67 +2201,71 @@
         <v>0.5</v>
       </c>
       <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" ht="142.5" customHeight="1">
+      <c r="A11" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="7">
+      <c r="B11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="2">
         <v>100</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="2">
         <v>100</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="2">
         <v>2</v>
       </c>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" ht="142.5" customHeight="1">
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" s="4" customFormat="1" ht="142.5" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I12" s="2">
         <v>200</v>
@@ -2070,103 +2277,109 @@
         <v>2</v>
       </c>
       <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" s="4" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="142.5" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2">
         <v>200</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="2">
         <v>100</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="2">
         <v>2</v>
       </c>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="142.5" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="142.5" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="7">
+      <c r="C14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="2">
         <v>50</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="2">
         <v>1000</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="2">
         <v>2</v>
       </c>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" ht="366">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="366">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I15" s="2">
         <v>100</v>
@@ -2176,57 +2389,75 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="366">
+      <c r="M15" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="366">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="366">
+        <v>96</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="2">
+        <v>100</v>
+      </c>
+      <c r="J16" s="2">
+        <v>200</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>5</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" ht="366">
       <c r="A17" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I17" s="2">
         <v>100</v>
@@ -2234,162 +2465,390 @@
       <c r="J17" s="2">
         <v>200</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
       <c r="L17" s="2">
+        <v>5</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" s="10" customFormat="1" ht="366">
+      <c r="A18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="7">
+        <v>100</v>
+      </c>
+      <c r="J18" s="7">
+        <v>200</v>
+      </c>
+      <c r="K18" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="366">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="L18" s="7">
+        <v>5</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" s="10" customFormat="1" ht="366">
+      <c r="A19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="7">
         <v>100</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2">
+      <c r="J19" s="7">
+        <v>200</v>
+      </c>
+      <c r="K19" s="7">
+        <v>2</v>
+      </c>
+      <c r="L19" s="7">
+        <v>2</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" s="4" customFormat="1" ht="396.75">
+      <c r="A20" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="13">
+        <v>23.59</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="13">
+        <v>100</v>
+      </c>
+      <c r="J20" s="13">
+        <v>200</v>
+      </c>
+      <c r="K20" s="13">
+        <v>2</v>
+      </c>
+      <c r="L20" s="13">
+        <v>50</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="351">
+      <c r="A21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="2">
+        <v>19.22</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="2">
+        <v>100</v>
+      </c>
+      <c r="J21" s="2">
+        <v>200</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2</v>
+      </c>
+      <c r="L21" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="396.75">
-      <c r="A19" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1.44</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="2">
-        <v>100</v>
-      </c>
-      <c r="J19" s="2">
-        <v>200</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="351">
-      <c r="A20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="2">
-        <v>20.440000000000001</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="2">
-        <v>100</v>
-      </c>
-      <c r="J20" s="2">
-        <v>200</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="366">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" ht="366">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" ht="321">
       <c r="A23" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="2">
+        <v>100</v>
+      </c>
+      <c r="J23" s="2">
+        <v>200</v>
+      </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="18" customFormat="1" ht="321">
+      <c r="A24" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="396.75">
+      <c r="A25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="2">
+        <v>17.07</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="2">
+        <v>100</v>
+      </c>
+      <c r="J25" s="2">
+        <v>200</v>
+      </c>
+      <c r="K25" s="2">
+        <v>2</v>
+      </c>
+      <c r="L25" s="2">
+        <v>5</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="60.75">
+      <c r="A26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" ht="366">
+      <c r="A27" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="16">
+        <v>100</v>
+      </c>
+      <c r="J27" s="16">
+        <v>200</v>
+      </c>
+      <c r="K27" s="16">
+        <v>2</v>
+      </c>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="18" customFormat="1" ht="209.25" customHeight="1">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2432,7 +2891,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -2449,25 +2908,25 @@
     </row>
     <row r="2" spans="1:9" ht="252" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3">
         <v>11.45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2">
         <v>100</v>
@@ -2478,25 +2937,25 @@
     </row>
     <row r="3" spans="1:9" ht="258" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="B3" s="3">
         <v>18.16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2">
         <v>100</v>
@@ -2507,25 +2966,25 @@
     </row>
     <row r="4" spans="1:9" ht="267.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B4" s="3">
         <v>18.329999999999998</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2">
         <v>1000</v>
@@ -2536,25 +2995,25 @@
     </row>
     <row r="5" spans="1:9" ht="106.5">
       <c r="A5" s="2" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3">
         <v>15.48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H5" s="2">
         <v>40</v>
@@ -2565,25 +3024,25 @@
     </row>
     <row r="6" spans="1:9" ht="306.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3">
         <v>20.329999999999998</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2">
         <v>50</v>
@@ -2594,25 +3053,25 @@
     </row>
     <row r="7" spans="1:9" ht="409.6">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="B7" s="3">
         <v>9.44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2">
         <v>100</v>
@@ -2623,25 +3082,25 @@
     </row>
     <row r="8" spans="1:9" ht="409.6">
       <c r="A8" s="2" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="B8" s="3">
         <v>22.54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H8" s="2">
         <v>150</v>
@@ -2652,25 +3111,25 @@
     </row>
     <row r="9" spans="1:9" ht="409.6">
       <c r="A9" s="2" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="B9" s="3">
         <v>20.190000000000001</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2">
         <v>200</v>
@@ -2684,7 +3143,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2694,23 +3153,23 @@
     </row>
     <row r="11" spans="1:9" ht="409.6">
       <c r="A11" s="2" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H11" s="2">
         <v>100</v>

</xml_diff>